<commit_message>
updated behavioral analysis, toproduce datasets for anova test in r
two way anova with repeated measurements isnt implemented in a python library
</commit_message>
<xml_diff>
--- a/REyeker-DataAnalyses-Python/results/data_of_all.xlsx
+++ b/REyeker-DataAnalyses-Python/results/data_of_all.xlsx
@@ -99,10 +99,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Top-Down</t>
+    <t>Bottom-Up</t>
   </si>
   <si>
-    <t>Bottom-Up</t>
+    <t>Top-Down</t>
   </si>
 </sst>
 </file>
@@ -17798,7 +17798,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18">
         <v>186</v>
@@ -17821,7 +17821,7 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19">
         <v>131</v>
@@ -17877,7 +17877,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>391</v>
@@ -17900,7 +17900,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>226</v>
@@ -17923,7 +17923,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>232</v>
@@ -17946,7 +17946,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>36</v>
@@ -17969,7 +17969,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>88</v>
@@ -17992,7 +17992,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>78</v>
@@ -18015,7 +18015,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>171</v>
@@ -18038,7 +18038,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9">
         <v>161</v>
@@ -18061,7 +18061,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>167</v>
@@ -18084,7 +18084,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>157</v>
@@ -18107,7 +18107,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>319</v>
@@ -18130,7 +18130,7 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>196</v>
@@ -18153,7 +18153,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>182</v>
@@ -18176,7 +18176,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>133</v>
@@ -18199,7 +18199,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>155</v>
@@ -18222,7 +18222,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17">
         <v>164</v>
@@ -18245,7 +18245,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18">
         <v>213</v>
@@ -18268,7 +18268,7 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19">
         <v>143</v>

</xml_diff>